<commit_message>
Linking multiple pages done
</commit_message>
<xml_diff>
--- a/data/dB.xlsx
+++ b/data/dB.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HCLTech_Dashboard\Temp_Database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HCLTech_Dashboard\Dashboard\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72AFBE79-1B7E-4B94-AF55-7D5D7028B46E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7736C8F0-7138-4202-9897-152D3AAADA67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-83" yWindow="0" windowWidth="14566" windowHeight="15563" xr2:uid="{9CAA6723-E93B-4360-9D44-745D8D6BCC11}"/>
+    <workbookView xWindow="2940" yWindow="2940" windowWidth="21600" windowHeight="11332" xr2:uid="{9CAA6723-E93B-4360-9D44-745D8D6BCC11}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -440,7 +440,7 @@
   <dimension ref="C3:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
Excel database connected with multiple screens. Now it can display all parameters based on the url
</commit_message>
<xml_diff>
--- a/data/dB.xlsx
+++ b/data/dB.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HCLTech_Dashboard\Dashboard\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7736C8F0-7138-4202-9897-152D3AAADA67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7160CE5E-728D-4C3F-853A-549BEC867DD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2940" yWindow="2940" windowWidth="21600" windowHeight="11332" xr2:uid="{9CAA6723-E93B-4360-9D44-745D8D6BCC11}"/>
+    <workbookView xWindow="2460" yWindow="3218" windowWidth="21600" windowHeight="11332" activeTab="1" xr2:uid="{9CAA6723-E93B-4360-9D44-745D8D6BCC11}"/>
   </bookViews>
   <sheets>
-    <sheet name="Blad1" sheetId="1" r:id="rId1"/>
+    <sheet name="Financials" sheetId="1" r:id="rId1"/>
+    <sheet name="Demand_view" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="10">
   <si>
     <t>id</t>
   </si>
@@ -437,87 +438,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2056A209-439C-471A-AC40-BB7C1896BCBF}">
-  <dimension ref="C3:I13"/>
+  <dimension ref="C6:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="3" spans="3:9" x14ac:dyDescent="0.45">
-      <c r="C3" t="s">
+    <row r="6" spans="3:9" x14ac:dyDescent="0.45">
+      <c r="C6" t="s">
         <v>0</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E6" t="s">
         <v>1</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G6" t="s">
         <v>2</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I6" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="3:9" x14ac:dyDescent="0.45">
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="E5" t="s">
-        <v>4</v>
-      </c>
-      <c r="G5">
-        <v>26</v>
-      </c>
-      <c r="I5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="3:9" x14ac:dyDescent="0.45">
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="E6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G6">
-        <v>28</v>
-      </c>
-      <c r="I6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="3:9" x14ac:dyDescent="0.45">
-      <c r="C7">
-        <v>3</v>
-      </c>
-      <c r="E7" t="s">
-        <v>6</v>
-      </c>
-      <c r="G7">
-        <v>108</v>
-      </c>
-      <c r="I7" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="8" spans="3:9" x14ac:dyDescent="0.45">
       <c r="C8">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E8" t="s">
         <v>4</v>
       </c>
       <c r="G8">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="3:9" x14ac:dyDescent="0.45">
       <c r="C9">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E9" t="s">
         <v>5</v>
@@ -526,12 +485,12 @@
         <v>28</v>
       </c>
       <c r="I9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="3:9" x14ac:dyDescent="0.45">
       <c r="C10">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E10" t="s">
         <v>6</v>
@@ -540,26 +499,26 @@
         <v>108</v>
       </c>
       <c r="I10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="3:9" x14ac:dyDescent="0.45">
       <c r="C11">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E11" t="s">
         <v>4</v>
       </c>
       <c r="G11">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="3:9" x14ac:dyDescent="0.45">
       <c r="C12">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E12" t="s">
         <v>5</v>
@@ -568,12 +527,12 @@
         <v>28</v>
       </c>
       <c r="I12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="3:9" x14ac:dyDescent="0.45">
       <c r="C13">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E13" t="s">
         <v>6</v>
@@ -582,6 +541,203 @@
         <v>108</v>
       </c>
       <c r="I13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="3:9" x14ac:dyDescent="0.45">
+      <c r="C14">
+        <v>7</v>
+      </c>
+      <c r="E14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G14">
+        <v>26</v>
+      </c>
+      <c r="I14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="3:9" x14ac:dyDescent="0.45">
+      <c r="C15">
+        <v>8</v>
+      </c>
+      <c r="E15" t="s">
+        <v>5</v>
+      </c>
+      <c r="G15">
+        <v>28</v>
+      </c>
+      <c r="I15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="3:9" x14ac:dyDescent="0.45">
+      <c r="C16">
+        <v>9</v>
+      </c>
+      <c r="E16" t="s">
+        <v>6</v>
+      </c>
+      <c r="G16">
+        <v>108</v>
+      </c>
+      <c r="I16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D8B6ABE-68B8-4414-B1AA-16F691A835FC}">
+  <dimension ref="D7:J17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="7" spans="4:10" x14ac:dyDescent="0.45">
+      <c r="D7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F7" t="s">
+        <v>1</v>
+      </c>
+      <c r="H7" t="s">
+        <v>2</v>
+      </c>
+      <c r="J7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="4:10" x14ac:dyDescent="0.45">
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9">
+        <v>3</v>
+      </c>
+      <c r="J9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="4:10" x14ac:dyDescent="0.45">
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="F10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10">
+        <v>2</v>
+      </c>
+      <c r="J10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="4:10" x14ac:dyDescent="0.45">
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="F11" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11">
+        <v>44</v>
+      </c>
+      <c r="J11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="4:10" x14ac:dyDescent="0.45">
+      <c r="D12">
+        <v>4</v>
+      </c>
+      <c r="F12" t="s">
+        <v>4</v>
+      </c>
+      <c r="H12">
+        <v>56</v>
+      </c>
+      <c r="J12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="4:10" x14ac:dyDescent="0.45">
+      <c r="D13">
+        <v>5</v>
+      </c>
+      <c r="F13" t="s">
+        <v>5</v>
+      </c>
+      <c r="H13">
+        <v>88</v>
+      </c>
+      <c r="J13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="4:10" x14ac:dyDescent="0.45">
+      <c r="D14">
+        <v>6</v>
+      </c>
+      <c r="F14" t="s">
+        <v>6</v>
+      </c>
+      <c r="H14">
+        <v>8</v>
+      </c>
+      <c r="J14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="4:10" x14ac:dyDescent="0.45">
+      <c r="D15">
+        <v>7</v>
+      </c>
+      <c r="F15" t="s">
+        <v>4</v>
+      </c>
+      <c r="H15">
+        <v>7</v>
+      </c>
+      <c r="J15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="4:10" x14ac:dyDescent="0.45">
+      <c r="D16">
+        <v>8</v>
+      </c>
+      <c r="F16" t="s">
+        <v>5</v>
+      </c>
+      <c r="H16">
+        <v>9</v>
+      </c>
+      <c r="J16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="4:10" x14ac:dyDescent="0.45">
+      <c r="D17">
+        <v>9</v>
+      </c>
+      <c r="F17" t="s">
+        <v>6</v>
+      </c>
+      <c r="H17">
+        <v>98</v>
+      </c>
+      <c r="J17" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Heading fixed and connected through database
</commit_message>
<xml_diff>
--- a/data/dB.xlsx
+++ b/data/dB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HCLTech_Dashboard\Dashboard\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0E345FC-3072-4994-B901-75023377E2E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0B23002-E605-43F2-8219-209C77C8B703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-660" yWindow="2033" windowWidth="21600" windowHeight="11332" activeTab="1" xr2:uid="{9CAA6723-E93B-4360-9D44-745D8D6BCC11}"/>
+    <workbookView xWindow="0" yWindow="2033" windowWidth="21600" windowHeight="11332" activeTab="1" xr2:uid="{9CAA6723-E93B-4360-9D44-745D8D6BCC11}"/>
   </bookViews>
   <sheets>
     <sheet name="Financials" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="17">
   <si>
     <t>id</t>
   </si>
@@ -82,16 +82,28 @@
   </si>
   <si>
     <t>Demand Count Vs Hackthon</t>
+  </si>
+  <si>
+    <t>heading</t>
+  </si>
+  <si>
+    <t>Total Revenue: 2023-2024</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -453,15 +465,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2056A209-439C-471A-AC40-BB7C1896BCBF}">
-  <dimension ref="C6:I16"/>
+  <dimension ref="C6:K16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:I16"/>
+      <selection activeCell="K6" sqref="K6:K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="6" spans="3:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C6" t="s">
         <v>0</v>
       </c>
@@ -474,8 +486,11 @@
       <c r="I6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="3:9" x14ac:dyDescent="0.45">
+      <c r="K6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C8">
         <v>1</v>
       </c>
@@ -488,8 +503,11 @@
       <c r="I8" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="3:9" x14ac:dyDescent="0.45">
+      <c r="K8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C9">
         <v>2</v>
       </c>
@@ -502,8 +520,11 @@
       <c r="I9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="3:9" x14ac:dyDescent="0.45">
+      <c r="K9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C10">
         <v>3</v>
       </c>
@@ -516,8 +537,11 @@
       <c r="I10" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="3:9" x14ac:dyDescent="0.45">
+      <c r="K10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C11">
         <v>4</v>
       </c>
@@ -530,8 +554,11 @@
       <c r="I11" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="12" spans="3:9" x14ac:dyDescent="0.45">
+      <c r="K11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C12">
         <v>5</v>
       </c>
@@ -544,8 +571,11 @@
       <c r="I12" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="3:9" x14ac:dyDescent="0.45">
+      <c r="K12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C13">
         <v>6</v>
       </c>
@@ -558,8 +588,11 @@
       <c r="I13" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="14" spans="3:9" x14ac:dyDescent="0.45">
+      <c r="K13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C14">
         <v>7</v>
       </c>
@@ -572,8 +605,11 @@
       <c r="I14" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="15" spans="3:9" x14ac:dyDescent="0.45">
+      <c r="K14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C15">
         <v>8</v>
       </c>
@@ -586,8 +622,11 @@
       <c r="I15" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="16" spans="3:9" x14ac:dyDescent="0.45">
+      <c r="K15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="3:11" x14ac:dyDescent="0.45">
       <c r="C16">
         <v>9</v>
       </c>
@@ -600,23 +639,27 @@
       <c r="I16" t="s">
         <v>9</v>
       </c>
+      <c r="K16" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D8B6ABE-68B8-4414-B1AA-16F691A835FC}">
-  <dimension ref="D7:J12"/>
+  <dimension ref="D7:M12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="7" spans="4:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="4:13" x14ac:dyDescent="0.45">
       <c r="D7" t="s">
         <v>0</v>
       </c>
@@ -629,8 +672,11 @@
       <c r="J7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="4:10" x14ac:dyDescent="0.45">
+      <c r="M7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="4:13" x14ac:dyDescent="0.45">
       <c r="D9">
         <v>1</v>
       </c>
@@ -640,8 +686,11 @@
       <c r="H9">
         <v>94</v>
       </c>
-    </row>
-    <row r="10" spans="4:10" x14ac:dyDescent="0.45">
+      <c r="M9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="4:13" x14ac:dyDescent="0.45">
       <c r="D10">
         <v>2</v>
       </c>
@@ -654,8 +703,11 @@
       <c r="J10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="4:10" x14ac:dyDescent="0.45">
+      <c r="M10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="4:13" x14ac:dyDescent="0.45">
       <c r="D11">
         <v>3</v>
       </c>
@@ -668,8 +720,11 @@
       <c r="J11" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="12" spans="4:10" x14ac:dyDescent="0.45">
+      <c r="M11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="4:13" x14ac:dyDescent="0.45">
       <c r="D12">
         <v>4</v>
       </c>
@@ -681,6 +736,9 @@
       </c>
       <c r="J12" t="s">
         <v>14</v>
+      </c>
+      <c r="M12" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Third page almost done
</commit_message>
<xml_diff>
--- a/data/dB.xlsx
+++ b/data/dB.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HCLTech_Dashboard\Dashboard\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0B23002-E605-43F2-8219-209C77C8B703}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1065F09-1C6A-4E94-9DA9-523A7DA2C886}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2033" windowWidth="21600" windowHeight="11332" activeTab="1" xr2:uid="{9CAA6723-E93B-4360-9D44-745D8D6BCC11}"/>
+    <workbookView xWindow="14317" yWindow="0" windowWidth="14565" windowHeight="15563" activeTab="2" xr2:uid="{9CAA6723-E93B-4360-9D44-745D8D6BCC11}"/>
   </bookViews>
   <sheets>
     <sheet name="Financials" sheetId="1" r:id="rId1"/>
     <sheet name="Demand_view" sheetId="2" r:id="rId2"/>
+    <sheet name="Fulfilment_view" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="23">
   <si>
     <t>id</t>
   </si>
@@ -88,6 +89,24 @@
   </si>
   <si>
     <t>Total Revenue: 2023-2024</t>
+  </si>
+  <si>
+    <t>Intial Net Billed Resources</t>
+  </si>
+  <si>
+    <t>No. Of External Fulfilment</t>
+  </si>
+  <si>
+    <t>No. Of Internal Fulfilment</t>
+  </si>
+  <si>
+    <t>Netbilled HC UPTICK</t>
+  </si>
+  <si>
+    <t>Total Demands Vs External Fulfilment</t>
+  </si>
+  <si>
+    <t>Total Demands Vs Internal Fulfilment</t>
   </si>
 </sst>
 </file>
@@ -653,8 +672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D8B6ABE-68B8-4414-B1AA-16F691A835FC}">
   <dimension ref="D7:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7:M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -744,4 +763,105 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{067B8890-6297-4A90-8406-A846D6520200}">
+  <dimension ref="D7:M12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="7" max="7" width="13.59765625" customWidth="1"/>
+    <col min="10" max="10" width="29.9296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="7" spans="4:13" x14ac:dyDescent="0.45">
+      <c r="D7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F7" t="s">
+        <v>1</v>
+      </c>
+      <c r="H7" t="s">
+        <v>2</v>
+      </c>
+      <c r="J7" t="s">
+        <v>3</v>
+      </c>
+      <c r="M7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="4:13" x14ac:dyDescent="0.45">
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9">
+        <v>94</v>
+      </c>
+      <c r="M9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="4:13" x14ac:dyDescent="0.45">
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="F10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10">
+        <v>76</v>
+      </c>
+      <c r="J10" t="s">
+        <v>20</v>
+      </c>
+      <c r="M10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="4:13" x14ac:dyDescent="0.45">
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="F11" t="s">
+        <v>18</v>
+      </c>
+      <c r="H11">
+        <v>50</v>
+      </c>
+      <c r="J11" t="s">
+        <v>21</v>
+      </c>
+      <c r="M11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="4:13" x14ac:dyDescent="0.45">
+      <c r="D12">
+        <v>4</v>
+      </c>
+      <c r="F12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12">
+        <v>26</v>
+      </c>
+      <c r="J12" t="s">
+        <v>22</v>
+      </c>
+      <c r="M12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
DB update for financials
</commit_message>
<xml_diff>
--- a/data/dB.xlsx
+++ b/data/dB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HCLTech_Dashboard\Dashboard\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6C1D3BD-A4B9-4E82-B3AA-909DAE48C0A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80D122CE-64CA-43D2-963B-A4D0C7870D3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-83" yWindow="0" windowWidth="14566" windowHeight="15563" activeTab="2" xr2:uid="{9CAA6723-E93B-4360-9D44-745D8D6BCC11}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{9CAA6723-E93B-4360-9D44-745D8D6BCC11}"/>
   </bookViews>
   <sheets>
     <sheet name="Financials" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="38">
   <si>
     <t>id</t>
   </si>
@@ -113,6 +113,45 @@
   </si>
   <si>
     <t>Fulfillment Chanel Performance</t>
+  </si>
+  <si>
+    <t>2020-2021</t>
+  </si>
+  <si>
+    <t>Onsite</t>
+  </si>
+  <si>
+    <t>UKISA</t>
+  </si>
+  <si>
+    <t>PERIOD</t>
+  </si>
+  <si>
+    <t>YEAR</t>
+  </si>
+  <si>
+    <t>CLUSTER</t>
+  </si>
+  <si>
+    <t>ACCOUNT NAME</t>
+  </si>
+  <si>
+    <t>LOCATION</t>
+  </si>
+  <si>
+    <t>Finastra</t>
+  </si>
+  <si>
+    <t>2021-2022</t>
+  </si>
+  <si>
+    <t>ERGER</t>
+  </si>
+  <si>
+    <t>GER</t>
+  </si>
+  <si>
+    <t>Offsite</t>
   </si>
 </sst>
 </file>
@@ -490,15 +529,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2056A209-439C-471A-AC40-BB7C1896BCBF}">
-  <dimension ref="C6:K16"/>
+  <dimension ref="C6:U34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K6" sqref="K6:K16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="5" max="5" width="18.3984375" customWidth="1"/>
+    <col min="11" max="11" width="22.265625" customWidth="1"/>
+    <col min="15" max="15" width="10.3984375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="6" spans="3:11" x14ac:dyDescent="0.45">
+    <row r="6" spans="3:21" x14ac:dyDescent="0.45">
       <c r="C6" t="s">
         <v>0</v>
       </c>
@@ -514,8 +558,23 @@
       <c r="K6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="3:11" x14ac:dyDescent="0.45">
+      <c r="M6" t="s">
+        <v>28</v>
+      </c>
+      <c r="O6" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>30</v>
+      </c>
+      <c r="S6" t="s">
+        <v>31</v>
+      </c>
+      <c r="U6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="3:21" x14ac:dyDescent="0.45">
       <c r="C8">
         <v>1</v>
       </c>
@@ -531,8 +590,23 @@
       <c r="K8" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="3:11" x14ac:dyDescent="0.45">
+      <c r="M8">
+        <v>2020</v>
+      </c>
+      <c r="O8" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>27</v>
+      </c>
+      <c r="S8" t="s">
+        <v>33</v>
+      </c>
+      <c r="U8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="3:21" x14ac:dyDescent="0.45">
       <c r="C9">
         <v>2</v>
       </c>
@@ -548,8 +622,23 @@
       <c r="K9" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="3:11" x14ac:dyDescent="0.45">
+      <c r="M9">
+        <v>2020</v>
+      </c>
+      <c r="O9" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>27</v>
+      </c>
+      <c r="S9" t="s">
+        <v>33</v>
+      </c>
+      <c r="U9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="3:21" x14ac:dyDescent="0.45">
       <c r="C10">
         <v>3</v>
       </c>
@@ -565,8 +654,23 @@
       <c r="K10" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="11" spans="3:11" x14ac:dyDescent="0.45">
+      <c r="M10">
+        <v>2020</v>
+      </c>
+      <c r="O10" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>27</v>
+      </c>
+      <c r="S10" t="s">
+        <v>33</v>
+      </c>
+      <c r="U10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="3:21" x14ac:dyDescent="0.45">
       <c r="C11">
         <v>4</v>
       </c>
@@ -582,8 +686,23 @@
       <c r="K11" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="12" spans="3:11" x14ac:dyDescent="0.45">
+      <c r="M11">
+        <v>2020</v>
+      </c>
+      <c r="O11" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>27</v>
+      </c>
+      <c r="S11" t="s">
+        <v>33</v>
+      </c>
+      <c r="U11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="3:21" x14ac:dyDescent="0.45">
       <c r="C12">
         <v>5</v>
       </c>
@@ -599,8 +718,23 @@
       <c r="K12" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="13" spans="3:11" x14ac:dyDescent="0.45">
+      <c r="M12">
+        <v>2020</v>
+      </c>
+      <c r="O12" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>27</v>
+      </c>
+      <c r="S12" t="s">
+        <v>33</v>
+      </c>
+      <c r="U12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="3:21" x14ac:dyDescent="0.45">
       <c r="C13">
         <v>6</v>
       </c>
@@ -616,8 +750,23 @@
       <c r="K13" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="14" spans="3:11" x14ac:dyDescent="0.45">
+      <c r="M13">
+        <v>2020</v>
+      </c>
+      <c r="O13" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>27</v>
+      </c>
+      <c r="S13" t="s">
+        <v>33</v>
+      </c>
+      <c r="U13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="3:21" x14ac:dyDescent="0.45">
       <c r="C14">
         <v>7</v>
       </c>
@@ -633,8 +782,23 @@
       <c r="K14" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="15" spans="3:11" x14ac:dyDescent="0.45">
+      <c r="M14">
+        <v>2020</v>
+      </c>
+      <c r="O14" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>27</v>
+      </c>
+      <c r="S14" t="s">
+        <v>33</v>
+      </c>
+      <c r="U14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="3:21" x14ac:dyDescent="0.45">
       <c r="C15">
         <v>8</v>
       </c>
@@ -650,8 +814,23 @@
       <c r="K15" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="16" spans="3:11" x14ac:dyDescent="0.45">
+      <c r="M15">
+        <v>2020</v>
+      </c>
+      <c r="O15" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>27</v>
+      </c>
+      <c r="S15" t="s">
+        <v>33</v>
+      </c>
+      <c r="U15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="3:21" x14ac:dyDescent="0.45">
       <c r="C16">
         <v>9</v>
       </c>
@@ -666,6 +845,341 @@
       </c>
       <c r="K16" t="s">
         <v>16</v>
+      </c>
+      <c r="M16">
+        <v>2020</v>
+      </c>
+      <c r="O16" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>27</v>
+      </c>
+      <c r="S16" t="s">
+        <v>33</v>
+      </c>
+      <c r="U16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="3:21" x14ac:dyDescent="0.45">
+      <c r="C24" t="s">
+        <v>0</v>
+      </c>
+      <c r="E24" t="s">
+        <v>1</v>
+      </c>
+      <c r="G24" t="s">
+        <v>2</v>
+      </c>
+      <c r="I24" t="s">
+        <v>3</v>
+      </c>
+      <c r="K24" t="s">
+        <v>15</v>
+      </c>
+      <c r="M24" t="s">
+        <v>28</v>
+      </c>
+      <c r="O24" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>30</v>
+      </c>
+      <c r="S24" t="s">
+        <v>31</v>
+      </c>
+      <c r="U24" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="3:21" x14ac:dyDescent="0.45">
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="E26" t="s">
+        <v>4</v>
+      </c>
+      <c r="G26">
+        <v>55</v>
+      </c>
+      <c r="I26" t="s">
+        <v>7</v>
+      </c>
+      <c r="K26" t="s">
+        <v>16</v>
+      </c>
+      <c r="M26">
+        <v>2021</v>
+      </c>
+      <c r="O26" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>35</v>
+      </c>
+      <c r="S26" t="s">
+        <v>36</v>
+      </c>
+      <c r="U26" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="3:21" x14ac:dyDescent="0.45">
+      <c r="C27">
+        <v>2</v>
+      </c>
+      <c r="E27" t="s">
+        <v>5</v>
+      </c>
+      <c r="G27">
+        <v>4</v>
+      </c>
+      <c r="I27" t="s">
+        <v>7</v>
+      </c>
+      <c r="K27" t="s">
+        <v>16</v>
+      </c>
+      <c r="M27">
+        <v>2021</v>
+      </c>
+      <c r="O27" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>35</v>
+      </c>
+      <c r="S27" t="s">
+        <v>36</v>
+      </c>
+      <c r="U27" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="3:21" x14ac:dyDescent="0.45">
+      <c r="C28">
+        <v>3</v>
+      </c>
+      <c r="E28" t="s">
+        <v>6</v>
+      </c>
+      <c r="G28">
+        <v>67</v>
+      </c>
+      <c r="I28" t="s">
+        <v>7</v>
+      </c>
+      <c r="K28" t="s">
+        <v>16</v>
+      </c>
+      <c r="M28">
+        <v>2021</v>
+      </c>
+      <c r="O28" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>35</v>
+      </c>
+      <c r="S28" t="s">
+        <v>36</v>
+      </c>
+      <c r="U28" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="3:21" x14ac:dyDescent="0.45">
+      <c r="C29">
+        <v>4</v>
+      </c>
+      <c r="E29" t="s">
+        <v>4</v>
+      </c>
+      <c r="G29">
+        <v>8</v>
+      </c>
+      <c r="I29" t="s">
+        <v>8</v>
+      </c>
+      <c r="K29" t="s">
+        <v>16</v>
+      </c>
+      <c r="M29">
+        <v>2021</v>
+      </c>
+      <c r="O29" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>35</v>
+      </c>
+      <c r="S29" t="s">
+        <v>36</v>
+      </c>
+      <c r="U29" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="3:21" x14ac:dyDescent="0.45">
+      <c r="C30">
+        <v>5</v>
+      </c>
+      <c r="E30" t="s">
+        <v>5</v>
+      </c>
+      <c r="G30">
+        <v>99</v>
+      </c>
+      <c r="I30" t="s">
+        <v>8</v>
+      </c>
+      <c r="K30" t="s">
+        <v>16</v>
+      </c>
+      <c r="M30">
+        <v>2021</v>
+      </c>
+      <c r="O30" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>35</v>
+      </c>
+      <c r="S30" t="s">
+        <v>36</v>
+      </c>
+      <c r="U30" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="3:21" x14ac:dyDescent="0.45">
+      <c r="C31">
+        <v>6</v>
+      </c>
+      <c r="E31" t="s">
+        <v>6</v>
+      </c>
+      <c r="G31">
+        <v>7</v>
+      </c>
+      <c r="I31" t="s">
+        <v>8</v>
+      </c>
+      <c r="K31" t="s">
+        <v>16</v>
+      </c>
+      <c r="M31">
+        <v>2021</v>
+      </c>
+      <c r="O31" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>35</v>
+      </c>
+      <c r="S31" t="s">
+        <v>36</v>
+      </c>
+      <c r="U31" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" spans="3:21" x14ac:dyDescent="0.45">
+      <c r="C32">
+        <v>7</v>
+      </c>
+      <c r="E32" t="s">
+        <v>4</v>
+      </c>
+      <c r="G32">
+        <v>56</v>
+      </c>
+      <c r="I32" t="s">
+        <v>9</v>
+      </c>
+      <c r="K32" t="s">
+        <v>16</v>
+      </c>
+      <c r="M32">
+        <v>2021</v>
+      </c>
+      <c r="O32" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>35</v>
+      </c>
+      <c r="S32" t="s">
+        <v>36</v>
+      </c>
+      <c r="U32" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="3:21" x14ac:dyDescent="0.45">
+      <c r="C33">
+        <v>8</v>
+      </c>
+      <c r="E33" t="s">
+        <v>5</v>
+      </c>
+      <c r="G33">
+        <v>32</v>
+      </c>
+      <c r="I33" t="s">
+        <v>9</v>
+      </c>
+      <c r="K33" t="s">
+        <v>16</v>
+      </c>
+      <c r="M33">
+        <v>2021</v>
+      </c>
+      <c r="O33" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>35</v>
+      </c>
+      <c r="S33" t="s">
+        <v>36</v>
+      </c>
+      <c r="U33" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="3:21" x14ac:dyDescent="0.45">
+      <c r="C34">
+        <v>9</v>
+      </c>
+      <c r="E34" t="s">
+        <v>6</v>
+      </c>
+      <c r="G34">
+        <v>67</v>
+      </c>
+      <c r="I34" t="s">
+        <v>9</v>
+      </c>
+      <c r="K34" t="s">
+        <v>16</v>
+      </c>
+      <c r="M34">
+        <v>2021</v>
+      </c>
+      <c r="O34" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>35</v>
+      </c>
+      <c r="S34" t="s">
+        <v>36</v>
+      </c>
+      <c r="U34" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -775,8 +1289,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{067B8890-6297-4A90-8406-A846D6520200}">
   <dimension ref="D7:M13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
Leadership screen add. Parameters not rendering
</commit_message>
<xml_diff>
--- a/data/dB.xlsx
+++ b/data/dB.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HCLTech_Dashboard\Dashboard\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E9318F8-77FE-4B31-BE1B-6450AFD60259}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFC13DE1-8EE3-4BB3-BDAB-929D8AFB0349}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1418" yWindow="2168" windowWidth="23940" windowHeight="13290" xr2:uid="{9CAA6723-E93B-4360-9D44-745D8D6BCC11}"/>
+    <workbookView xWindow="1980" yWindow="2175" windowWidth="23940" windowHeight="13290" activeTab="3" xr2:uid="{9CAA6723-E93B-4360-9D44-745D8D6BCC11}"/>
   </bookViews>
   <sheets>
     <sheet name="Financials" sheetId="1" r:id="rId1"/>
     <sheet name="Demand_view" sheetId="2" r:id="rId2"/>
     <sheet name="Fulfilment_view" sheetId="3" r:id="rId3"/>
+    <sheet name="Thought_leadership_demonstratio" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="45">
   <si>
     <t>id</t>
   </si>
@@ -552,7 +553,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2056A209-439C-471A-AC40-BB7C1896BCBF}">
   <dimension ref="C6:U51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E25" workbookViewId="0">
+    <sheetView topLeftCell="E25" workbookViewId="0">
       <selection activeCell="V41" sqref="V41"/>
     </sheetView>
   </sheetViews>
@@ -1631,7 +1632,7 @@
   <dimension ref="D7:M13"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+      <selection activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1737,4 +1738,118 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CB0321B-1694-4805-B7CB-5AE863A01116}">
+  <dimension ref="C6:L12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="5" max="5" width="38" customWidth="1"/>
+    <col min="6" max="6" width="8.796875" customWidth="1"/>
+    <col min="9" max="9" width="30.6640625" customWidth="1"/>
+    <col min="12" max="12" width="22.265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="3:12" x14ac:dyDescent="0.45">
+      <c r="C6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>2</v>
+      </c>
+      <c r="I6" t="s">
+        <v>3</v>
+      </c>
+      <c r="L6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="3:12" x14ac:dyDescent="0.45">
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8">
+        <v>45</v>
+      </c>
+      <c r="L8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="3:12" x14ac:dyDescent="0.45">
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9">
+        <v>45</v>
+      </c>
+      <c r="I9" t="s">
+        <v>20</v>
+      </c>
+      <c r="L9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="3:12" x14ac:dyDescent="0.45">
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="E10" t="s">
+        <v>23</v>
+      </c>
+      <c r="I10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="3:12" x14ac:dyDescent="0.45">
+      <c r="C11">
+        <v>4</v>
+      </c>
+      <c r="E11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11">
+        <v>33</v>
+      </c>
+      <c r="I11" t="s">
+        <v>21</v>
+      </c>
+      <c r="L11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="3:12" x14ac:dyDescent="0.45">
+      <c r="C12">
+        <v>5</v>
+      </c>
+      <c r="E12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G12">
+        <v>99</v>
+      </c>
+      <c r="I12" t="s">
+        <v>22</v>
+      </c>
+      <c r="L12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
North Star POD page done
</commit_message>
<xml_diff>
--- a/data/dB.xlsx
+++ b/data/dB.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HCLTech_Dashboard\Dashboard\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0E287A4-64D8-46E4-B81F-AE1F4D1BBE0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC8D6632-91AA-4729-A3D2-6071E0173555}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="2175" windowWidth="23940" windowHeight="13290" activeTab="3" xr2:uid="{9CAA6723-E93B-4360-9D44-745D8D6BCC11}"/>
+    <workbookView xWindow="14317" yWindow="0" windowWidth="14565" windowHeight="15563" activeTab="4" xr2:uid="{9CAA6723-E93B-4360-9D44-745D8D6BCC11}"/>
   </bookViews>
   <sheets>
     <sheet name="Financials" sheetId="1" r:id="rId1"/>
     <sheet name="Demand_view" sheetId="2" r:id="rId2"/>
     <sheet name="Fulfilment_view" sheetId="3" r:id="rId3"/>
     <sheet name="Thought_leadership" sheetId="4" r:id="rId4"/>
+    <sheet name="North_star" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="56">
   <si>
     <t>id</t>
   </si>
@@ -192,6 +193,21 @@
   </si>
   <si>
     <t>40$ of Ideas converted as EN</t>
+  </si>
+  <si>
+    <t>Value Per Quarter</t>
+  </si>
+  <si>
+    <t>EN $</t>
+  </si>
+  <si>
+    <t>Measured in $ Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customer Value ADD - </t>
+  </si>
+  <si>
+    <t>Attrition %</t>
   </si>
 </sst>
 </file>
@@ -1762,8 +1778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CB0321B-1694-4805-B7CB-5AE863A01116}">
   <dimension ref="C16:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16:L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1837,4 +1853,84 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5C7C0CD-5A0A-4AB9-A8FE-8201FB8719E1}">
+  <dimension ref="E14:N18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="Q17" sqref="Q17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="14" spans="5:14" x14ac:dyDescent="0.45">
+      <c r="E14" t="s">
+        <v>0</v>
+      </c>
+      <c r="G14" t="s">
+        <v>1</v>
+      </c>
+      <c r="I14" t="s">
+        <v>2</v>
+      </c>
+      <c r="K14" t="s">
+        <v>3</v>
+      </c>
+      <c r="N14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="5:14" x14ac:dyDescent="0.45">
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="G16" t="s">
+        <v>51</v>
+      </c>
+      <c r="I16">
+        <v>76</v>
+      </c>
+      <c r="K16" t="s">
+        <v>52</v>
+      </c>
+      <c r="N16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="5:14" x14ac:dyDescent="0.45">
+      <c r="E17">
+        <v>2</v>
+      </c>
+      <c r="G17" t="s">
+        <v>53</v>
+      </c>
+      <c r="I17">
+        <v>76</v>
+      </c>
+      <c r="K17" t="s">
+        <v>54</v>
+      </c>
+      <c r="N17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="5:14" x14ac:dyDescent="0.45">
+      <c r="E18">
+        <v>3</v>
+      </c>
+      <c r="G18" t="s">
+        <v>55</v>
+      </c>
+      <c r="I18">
+        <v>60</v>
+      </c>
+      <c r="N18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
HCLTech specific page done
</commit_message>
<xml_diff>
--- a/data/dB.xlsx
+++ b/data/dB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HCLTech_Dashboard\Dashboard\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10C94F41-6F40-4E28-8DFE-1F3FC427ED28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0FC903D-26F7-420E-947D-0978DD3617D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14317" yWindow="0" windowWidth="14565" windowHeight="15563" activeTab="5" xr2:uid="{9CAA6723-E93B-4360-9D44-745D8D6BCC11}"/>
+    <workbookView xWindow="14317" yWindow="0" windowWidth="14565" windowHeight="15563" activeTab="6" xr2:uid="{9CAA6723-E93B-4360-9D44-745D8D6BCC11}"/>
   </bookViews>
   <sheets>
     <sheet name="Financials" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Thought_leadership" sheetId="4" r:id="rId4"/>
     <sheet name="North_star" sheetId="5" r:id="rId5"/>
     <sheet name="GTM_improvement" sheetId="6" r:id="rId6"/>
+    <sheet name="Operations_hcltech" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="62">
   <si>
     <t>id</t>
   </si>
@@ -218,6 +219,15 @@
   </si>
   <si>
     <t>FTE Count Increased</t>
+  </si>
+  <si>
+    <t>AVG. RESOURCE COST</t>
+  </si>
+  <si>
+    <t>UTILISATION %</t>
+  </si>
+  <si>
+    <t>something</t>
   </si>
 </sst>
 </file>
@@ -1949,8 +1959,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48201469-AAFD-45E5-9709-A98526EE2BE7}">
   <dimension ref="F14:O18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14:O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2017,4 +2027,78 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C54E2ED4-78AC-4FA7-B729-F0C6DF47B945}">
+  <dimension ref="E12:N16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="12" spans="5:14" x14ac:dyDescent="0.45">
+      <c r="E12" t="s">
+        <v>0</v>
+      </c>
+      <c r="G12" t="s">
+        <v>1</v>
+      </c>
+      <c r="I12" t="s">
+        <v>2</v>
+      </c>
+      <c r="K12" t="s">
+        <v>3</v>
+      </c>
+      <c r="N12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="5:14" x14ac:dyDescent="0.45">
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
+        <v>59</v>
+      </c>
+      <c r="I14">
+        <v>76</v>
+      </c>
+      <c r="N14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="5:14" x14ac:dyDescent="0.45">
+      <c r="E15">
+        <v>2</v>
+      </c>
+      <c r="G15" t="s">
+        <v>60</v>
+      </c>
+      <c r="I15">
+        <v>76</v>
+      </c>
+      <c r="N15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="5:14" x14ac:dyDescent="0.45">
+      <c r="E16">
+        <v>3</v>
+      </c>
+      <c r="G16" t="s">
+        <v>61</v>
+      </c>
+      <c r="I16">
+        <v>60</v>
+      </c>
+      <c r="N16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Customer Delight page done
</commit_message>
<xml_diff>
--- a/data/dB.xlsx
+++ b/data/dB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HCLTech_Dashboard\Dashboard\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{697531A4-366F-49BC-B050-2BA1DFA1DE7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50C0E99A-4DDA-4837-ACC8-80069C5F4BE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="75" yWindow="113" windowWidth="23940" windowHeight="13290" activeTab="6" xr2:uid="{9CAA6723-E93B-4360-9D44-745D8D6BCC11}"/>
+    <workbookView xWindow="-83" yWindow="0" windowWidth="14566" windowHeight="15563" firstSheet="3" activeTab="7" xr2:uid="{9CAA6723-E93B-4360-9D44-745D8D6BCC11}"/>
   </bookViews>
   <sheets>
     <sheet name="Financials" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="North_star" sheetId="5" r:id="rId5"/>
     <sheet name="GTM_improvement" sheetId="6" r:id="rId6"/>
     <sheet name="Operations_hcltech" sheetId="7" r:id="rId7"/>
+    <sheet name="Customer_delight" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="64">
   <si>
     <t>id</t>
   </si>
@@ -152,12 +153,6 @@
     <t>ERGER</t>
   </si>
   <si>
-    <t>GER</t>
-  </si>
-  <si>
-    <t>Offsite</t>
-  </si>
-  <si>
     <t>Total Revenue: 2020-2021</t>
   </si>
   <si>
@@ -173,12 +168,6 @@
     <t>test</t>
   </si>
   <si>
-    <t>testen</t>
-  </si>
-  <si>
-    <t>Hybrid</t>
-  </si>
-  <si>
     <t>Monthly</t>
   </si>
   <si>
@@ -228,6 +217,24 @@
   </si>
   <si>
     <t>something</t>
+  </si>
+  <si>
+    <t>EBRD</t>
+  </si>
+  <si>
+    <t>Offshore</t>
+  </si>
+  <si>
+    <t>Nearshore</t>
+  </si>
+  <si>
+    <t>HSBC</t>
+  </si>
+  <si>
+    <t>ACSAT</t>
+  </si>
+  <si>
+    <t>PCSAT</t>
   </si>
 </sst>
 </file>
@@ -607,8 +614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2056A209-439C-471A-AC40-BB7C1896BCBF}">
   <dimension ref="C6:U51"/>
   <sheetViews>
-    <sheetView topLeftCell="E25" workbookViewId="0">
-      <selection activeCell="V41" sqref="V41"/>
+    <sheetView topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="S43" sqref="S43:S51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -664,7 +671,7 @@
         <v>7</v>
       </c>
       <c r="K8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="M8">
         <v>2020</v>
@@ -696,7 +703,7 @@
         <v>7</v>
       </c>
       <c r="K9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="M9">
         <v>2020</v>
@@ -728,7 +735,7 @@
         <v>7</v>
       </c>
       <c r="K10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="M10">
         <v>2020</v>
@@ -760,7 +767,7 @@
         <v>8</v>
       </c>
       <c r="K11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="M11">
         <v>2020</v>
@@ -792,7 +799,7 @@
         <v>8</v>
       </c>
       <c r="K12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="M12">
         <v>2020</v>
@@ -824,7 +831,7 @@
         <v>8</v>
       </c>
       <c r="K13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="M13">
         <v>2020</v>
@@ -856,7 +863,7 @@
         <v>9</v>
       </c>
       <c r="K14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="M14">
         <v>2020</v>
@@ -888,7 +895,7 @@
         <v>9</v>
       </c>
       <c r="K15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="M15">
         <v>2020</v>
@@ -920,7 +927,7 @@
         <v>9</v>
       </c>
       <c r="K16" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="M16">
         <v>2020</v>
@@ -984,7 +991,7 @@
         <v>7</v>
       </c>
       <c r="K26" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="M26">
         <v>2021</v>
@@ -996,10 +1003,10 @@
         <v>35</v>
       </c>
       <c r="S26" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="U26" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
     </row>
     <row r="27" spans="3:21" x14ac:dyDescent="0.45">
@@ -1016,7 +1023,7 @@
         <v>7</v>
       </c>
       <c r="K27" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="M27">
         <v>2021</v>
@@ -1028,10 +1035,10 @@
         <v>35</v>
       </c>
       <c r="S27" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="U27" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="3:21" x14ac:dyDescent="0.45">
@@ -1048,7 +1055,7 @@
         <v>7</v>
       </c>
       <c r="K28" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="M28">
         <v>2021</v>
@@ -1060,10 +1067,10 @@
         <v>35</v>
       </c>
       <c r="S28" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="U28" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
     </row>
     <row r="29" spans="3:21" x14ac:dyDescent="0.45">
@@ -1080,7 +1087,7 @@
         <v>8</v>
       </c>
       <c r="K29" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="M29">
         <v>2021</v>
@@ -1092,10 +1099,10 @@
         <v>35</v>
       </c>
       <c r="S29" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="U29" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
     </row>
     <row r="30" spans="3:21" x14ac:dyDescent="0.45">
@@ -1112,7 +1119,7 @@
         <v>8</v>
       </c>
       <c r="K30" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="M30">
         <v>2021</v>
@@ -1124,10 +1131,10 @@
         <v>35</v>
       </c>
       <c r="S30" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="U30" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
     </row>
     <row r="31" spans="3:21" x14ac:dyDescent="0.45">
@@ -1144,7 +1151,7 @@
         <v>8</v>
       </c>
       <c r="K31" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="M31">
         <v>2021</v>
@@ -1156,10 +1163,10 @@
         <v>35</v>
       </c>
       <c r="S31" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="U31" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
     </row>
     <row r="32" spans="3:21" x14ac:dyDescent="0.45">
@@ -1176,7 +1183,7 @@
         <v>9</v>
       </c>
       <c r="K32" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="M32">
         <v>2021</v>
@@ -1188,10 +1195,10 @@
         <v>35</v>
       </c>
       <c r="S32" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="U32" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
     </row>
     <row r="33" spans="3:21" x14ac:dyDescent="0.45">
@@ -1208,7 +1215,7 @@
         <v>9</v>
       </c>
       <c r="K33" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="M33">
         <v>2021</v>
@@ -1220,10 +1227,10 @@
         <v>35</v>
       </c>
       <c r="S33" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="U33" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
     </row>
     <row r="34" spans="3:21" x14ac:dyDescent="0.45">
@@ -1240,7 +1247,7 @@
         <v>9</v>
       </c>
       <c r="K34" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="M34">
         <v>2021</v>
@@ -1252,10 +1259,10 @@
         <v>35</v>
       </c>
       <c r="S34" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="U34" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
     </row>
     <row r="41" spans="3:21" x14ac:dyDescent="0.45">
@@ -1304,22 +1311,22 @@
         <v>7</v>
       </c>
       <c r="K43" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="M43">
         <v>2022</v>
       </c>
       <c r="O43" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="Q43" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="S43" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="U43" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
     </row>
     <row r="44" spans="3:21" x14ac:dyDescent="0.45">
@@ -1336,22 +1343,22 @@
         <v>7</v>
       </c>
       <c r="K44" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="M44">
         <v>2022</v>
       </c>
       <c r="O44" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="Q44" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="S44" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="U44" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
     </row>
     <row r="45" spans="3:21" x14ac:dyDescent="0.45">
@@ -1368,22 +1375,22 @@
         <v>7</v>
       </c>
       <c r="K45" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="M45">
         <v>2022</v>
       </c>
       <c r="O45" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="Q45" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="S45" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="U45" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
     </row>
     <row r="46" spans="3:21" x14ac:dyDescent="0.45">
@@ -1400,22 +1407,22 @@
         <v>8</v>
       </c>
       <c r="K46" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="M46">
         <v>2022</v>
       </c>
       <c r="O46" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="Q46" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="S46" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="U46" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
     </row>
     <row r="47" spans="3:21" x14ac:dyDescent="0.45">
@@ -1432,22 +1439,22 @@
         <v>8</v>
       </c>
       <c r="K47" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="M47">
         <v>2022</v>
       </c>
       <c r="O47" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="Q47" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="S47" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="U47" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
     </row>
     <row r="48" spans="3:21" x14ac:dyDescent="0.45">
@@ -1464,22 +1471,22 @@
         <v>8</v>
       </c>
       <c r="K48" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="M48">
         <v>2022</v>
       </c>
       <c r="O48" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="Q48" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="S48" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="U48" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
     </row>
     <row r="49" spans="3:21" x14ac:dyDescent="0.45">
@@ -1496,22 +1503,22 @@
         <v>9</v>
       </c>
       <c r="K49" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="M49">
         <v>2022</v>
       </c>
       <c r="O49" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="Q49" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="S49" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="U49" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
     </row>
     <row r="50" spans="3:21" x14ac:dyDescent="0.45">
@@ -1528,22 +1535,22 @@
         <v>9</v>
       </c>
       <c r="K50" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="M50">
         <v>2022</v>
       </c>
       <c r="O50" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="Q50" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="S50" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="U50" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
     </row>
     <row r="51" spans="3:21" x14ac:dyDescent="0.45">
@@ -1560,22 +1567,22 @@
         <v>9</v>
       </c>
       <c r="K51" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="M51">
         <v>2022</v>
       </c>
       <c r="O51" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="Q51" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="S51" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="U51" t="s">
-        <v>44</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1832,13 +1839,13 @@
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="G18">
         <v>76</v>
       </c>
       <c r="I18" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="3:9" x14ac:dyDescent="0.45">
@@ -1846,13 +1853,13 @@
         <v>2</v>
       </c>
       <c r="E19" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G19">
         <v>47</v>
       </c>
       <c r="I19" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="3:9" x14ac:dyDescent="0.45">
@@ -1860,13 +1867,13 @@
         <v>3</v>
       </c>
       <c r="E20" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G20">
         <v>6</v>
       </c>
       <c r="I20" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1907,13 +1914,13 @@
         <v>1</v>
       </c>
       <c r="G16" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="I16">
         <v>76</v>
       </c>
       <c r="K16" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="N16" t="s">
         <v>16</v>
@@ -1924,13 +1931,13 @@
         <v>2</v>
       </c>
       <c r="G17" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="I17">
         <v>76</v>
       </c>
       <c r="K17" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="N17" t="s">
         <v>16</v>
@@ -1941,7 +1948,7 @@
         <v>3</v>
       </c>
       <c r="G18" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="I18">
         <v>60</v>
@@ -1987,7 +1994,7 @@
         <v>1</v>
       </c>
       <c r="H16" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="J16">
         <v>76</v>
@@ -2001,7 +2008,7 @@
         <v>2</v>
       </c>
       <c r="H17" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="J17">
         <v>76</v>
@@ -2015,7 +2022,7 @@
         <v>3</v>
       </c>
       <c r="H18" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="J18">
         <v>80</v>
@@ -2033,8 +2040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C54E2ED4-78AC-4FA7-B729-F0C6DF47B945}">
   <dimension ref="E12:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12:N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2061,7 +2068,7 @@
         <v>1</v>
       </c>
       <c r="G14" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="I14">
         <v>76</v>
@@ -2075,7 +2082,7 @@
         <v>2</v>
       </c>
       <c r="G15" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="I15">
         <v>76</v>
@@ -2089,12 +2096,72 @@
         <v>3</v>
       </c>
       <c r="G16" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="I16">
         <v>60</v>
       </c>
       <c r="N16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44332FF3-929A-46EC-9CF8-88538010FE32}">
+  <dimension ref="C11:L14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="11" spans="3:12" x14ac:dyDescent="0.45">
+      <c r="C11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>2</v>
+      </c>
+      <c r="I11" t="s">
+        <v>3</v>
+      </c>
+      <c r="L11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="3:12" x14ac:dyDescent="0.45">
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>62</v>
+      </c>
+      <c r="G13">
+        <v>85</v>
+      </c>
+      <c r="L13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="3:12" x14ac:dyDescent="0.45">
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="E14" t="s">
+        <v>63</v>
+      </c>
+      <c r="G14">
+        <v>6.3</v>
+      </c>
+      <c r="L14" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Engineer Delight page done
</commit_message>
<xml_diff>
--- a/data/dB.xlsx
+++ b/data/dB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HCLTech_Dashboard\Dashboard\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C02C5C80-2055-46BC-BCCB-9EA89EFF51B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BE0605A-D233-4F8E-BAC2-DAA7E7021CBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{9CAA6723-E93B-4360-9D44-745D8D6BCC11}"/>
+    <workbookView xWindow="14317" yWindow="0" windowWidth="14565" windowHeight="15563" firstSheet="2" activeTab="8" xr2:uid="{9CAA6723-E93B-4360-9D44-745D8D6BCC11}"/>
   </bookViews>
   <sheets>
     <sheet name="Financials" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="GTM_improvement" sheetId="6" r:id="rId6"/>
     <sheet name="Operations_hcltech" sheetId="7" r:id="rId7"/>
     <sheet name="Customer_delight" sheetId="8" r:id="rId8"/>
+    <sheet name="Engineer_delight" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="68">
   <si>
     <t>id</t>
   </si>
@@ -235,6 +236,18 @@
   </si>
   <si>
     <t>PCSAT</t>
+  </si>
+  <si>
+    <t>% of SOW Engineering Kitty</t>
+  </si>
+  <si>
+    <t>BRE Uptick Engineer</t>
+  </si>
+  <si>
+    <t>Employee Happiness Index</t>
+  </si>
+  <si>
+    <t>% of Lead Generated</t>
   </si>
 </sst>
 </file>
@@ -614,7 +627,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2056A209-439C-471A-AC40-BB7C1896BCBF}">
   <dimension ref="C6:U51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
@@ -2115,7 +2128,7 @@
   <dimension ref="C11:L14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="C11" sqref="C11:L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2168,4 +2181,93 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{845E186F-23E9-4636-B7BB-F09ADFC155D4}">
+  <dimension ref="E12:N17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16:K17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="12" spans="5:14" x14ac:dyDescent="0.45">
+      <c r="E12" t="s">
+        <v>0</v>
+      </c>
+      <c r="G12" t="s">
+        <v>1</v>
+      </c>
+      <c r="I12" t="s">
+        <v>2</v>
+      </c>
+      <c r="K12" t="s">
+        <v>3</v>
+      </c>
+      <c r="N12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="5:14" x14ac:dyDescent="0.45">
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
+        <v>64</v>
+      </c>
+      <c r="I14">
+        <v>76</v>
+      </c>
+      <c r="N14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="5:14" x14ac:dyDescent="0.45">
+      <c r="E15">
+        <v>2</v>
+      </c>
+      <c r="G15" t="s">
+        <v>65</v>
+      </c>
+      <c r="I15">
+        <v>76</v>
+      </c>
+      <c r="N15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="5:14" x14ac:dyDescent="0.45">
+      <c r="E16">
+        <v>3</v>
+      </c>
+      <c r="G16" t="s">
+        <v>66</v>
+      </c>
+      <c r="I16">
+        <v>60</v>
+      </c>
+      <c r="N16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="5:14" x14ac:dyDescent="0.45">
+      <c r="E17">
+        <v>4</v>
+      </c>
+      <c r="G17" t="s">
+        <v>67</v>
+      </c>
+      <c r="I17">
+        <v>60</v>
+      </c>
+      <c r="N17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Engineer Upskilling page done
</commit_message>
<xml_diff>
--- a/data/dB.xlsx
+++ b/data/dB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HCLTech_Dashboard\Dashboard\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{736EE596-1C8F-4155-9E9D-DA9E01164C41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D56F983-83AC-447F-A926-99C31AE62540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14317" yWindow="0" windowWidth="14565" windowHeight="15563" firstSheet="2" activeTab="8" xr2:uid="{9CAA6723-E93B-4360-9D44-745D8D6BCC11}"/>
+    <workbookView xWindow="2242" yWindow="1792" windowWidth="23940" windowHeight="13290" firstSheet="4" activeTab="9" xr2:uid="{9CAA6723-E93B-4360-9D44-745D8D6BCC11}"/>
   </bookViews>
   <sheets>
     <sheet name="Financials" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="Operations_hcltech" sheetId="7" r:id="rId7"/>
     <sheet name="Customer_delight" sheetId="8" r:id="rId8"/>
     <sheet name="Engineer_delight" sheetId="9" r:id="rId9"/>
+    <sheet name="Engineer_upskilling" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="71">
   <si>
     <t>id</t>
   </si>
@@ -248,6 +249,15 @@
   </si>
   <si>
     <t>% of Lead Generated</t>
+  </si>
+  <si>
+    <t>WHITE PAPERS</t>
+  </si>
+  <si>
+    <t>Joint Session with Customer</t>
+  </si>
+  <si>
+    <t>Upskilling/Cross Skilling - Based On Accound Categeration</t>
   </si>
 </sst>
 </file>
@@ -1604,6 +1614,80 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65648BBE-0CD0-4610-BC69-5EEC5DB552DD}">
+  <dimension ref="F14:O18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="14" spans="6:15" x14ac:dyDescent="0.45">
+      <c r="F14" t="s">
+        <v>0</v>
+      </c>
+      <c r="H14" t="s">
+        <v>1</v>
+      </c>
+      <c r="J14" t="s">
+        <v>2</v>
+      </c>
+      <c r="L14" t="s">
+        <v>3</v>
+      </c>
+      <c r="O14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="6:15" x14ac:dyDescent="0.45">
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="H16" t="s">
+        <v>68</v>
+      </c>
+      <c r="J16">
+        <v>77</v>
+      </c>
+      <c r="O16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="6:15" x14ac:dyDescent="0.45">
+      <c r="F17">
+        <v>2</v>
+      </c>
+      <c r="H17" t="s">
+        <v>69</v>
+      </c>
+      <c r="J17">
+        <v>58</v>
+      </c>
+      <c r="O17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="6:15" x14ac:dyDescent="0.45">
+      <c r="F18">
+        <v>3</v>
+      </c>
+      <c r="H18" t="s">
+        <v>70</v>
+      </c>
+      <c r="J18">
+        <v>90</v>
+      </c>
+      <c r="O18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D8B6ABE-68B8-4414-B1AA-16F691A835FC}">
   <dimension ref="D7:M12"/>
@@ -2187,8 +2271,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{845E186F-23E9-4636-B7BB-F09ADFC155D4}">
   <dimension ref="E12:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16:K17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12:N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
Governance Customer page done.
To Do:

Fix layout issue of Main14
</commit_message>
<xml_diff>
--- a/data/dB.xlsx
+++ b/data/dB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HCLTech_Dashboard\Dashboard\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D56F983-83AC-447F-A926-99C31AE62540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84B3C38E-3723-4A3E-92BB-8625E4D85DD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2242" yWindow="1792" windowWidth="23940" windowHeight="13290" firstSheet="4" activeTab="9" xr2:uid="{9CAA6723-E93B-4360-9D44-745D8D6BCC11}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" firstSheet="4" activeTab="10" xr2:uid="{9CAA6723-E93B-4360-9D44-745D8D6BCC11}"/>
   </bookViews>
   <sheets>
     <sheet name="Financials" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="Customer_delight" sheetId="8" r:id="rId8"/>
     <sheet name="Engineer_delight" sheetId="9" r:id="rId9"/>
     <sheet name="Engineer_upskilling" sheetId="10" r:id="rId10"/>
+    <sheet name="Governance_customer" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="72">
   <si>
     <t>id</t>
   </si>
@@ -258,6 +259,9 @@
   </si>
   <si>
     <t>Upskilling/Cross Skilling - Based On Accound Categeration</t>
+  </si>
+  <si>
+    <t>Count of Fortnightly Review</t>
   </si>
 </sst>
 </file>
@@ -1618,8 +1622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65648BBE-0CD0-4610-BC69-5EEC5DB552DD}">
   <dimension ref="F14:O18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14:O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1680,6 +1684,52 @@
         <v>90</v>
       </c>
       <c r="O18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94DD81D7-D221-42C9-849F-73FC0AD4452F}">
+  <dimension ref="F14:O16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="14" spans="6:15" x14ac:dyDescent="0.45">
+      <c r="F14" t="s">
+        <v>0</v>
+      </c>
+      <c r="H14" t="s">
+        <v>1</v>
+      </c>
+      <c r="J14" t="s">
+        <v>2</v>
+      </c>
+      <c r="L14" t="s">
+        <v>3</v>
+      </c>
+      <c r="O14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="6:15" x14ac:dyDescent="0.45">
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="H16" t="s">
+        <v>71</v>
+      </c>
+      <c r="J16">
+        <v>77</v>
+      </c>
+      <c r="O16" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Client Partner Focus done! Without ss
</commit_message>
<xml_diff>
--- a/data/dB.xlsx
+++ b/data/dB.xlsx
@@ -1,29 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HCLTech_Dashboard\Dashboard\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brahamjeet/HCLTech_Dashboard/Dashboard/Dashboard-HCLTech/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26ECC35C-C19B-4AD4-8893-38024386773E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{797E32F8-E407-3C40-ABBA-2FAA64F0AA36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14317" yWindow="0" windowWidth="14565" windowHeight="15563" xr2:uid="{9CAA6723-E93B-4360-9D44-745D8D6BCC11}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="3" xr2:uid="{9CAA6723-E93B-4360-9D44-745D8D6BCC11}"/>
   </bookViews>
   <sheets>
     <sheet name="Financials" sheetId="1" r:id="rId1"/>
     <sheet name="Demand_view" sheetId="2" r:id="rId2"/>
     <sheet name="Fulfilment_view" sheetId="3" r:id="rId3"/>
-    <sheet name="Thought_leadership" sheetId="4" r:id="rId4"/>
-    <sheet name="North_star" sheetId="5" r:id="rId5"/>
-    <sheet name="GTM_improvement" sheetId="6" r:id="rId6"/>
-    <sheet name="Operations_hcltech" sheetId="7" r:id="rId7"/>
-    <sheet name="Customer_delight" sheetId="8" r:id="rId8"/>
-    <sheet name="Engineer_delight" sheetId="9" r:id="rId9"/>
-    <sheet name="Engineer_upskilling" sheetId="10" r:id="rId10"/>
-    <sheet name="Governance_customer" sheetId="11" r:id="rId11"/>
+    <sheet name="Client_partner" sheetId="12" r:id="rId4"/>
+    <sheet name="Thought_leadership" sheetId="4" r:id="rId5"/>
+    <sheet name="North_star" sheetId="5" r:id="rId6"/>
+    <sheet name="GTM_improvement" sheetId="6" r:id="rId7"/>
+    <sheet name="Operations_hcltech" sheetId="7" r:id="rId8"/>
+    <sheet name="Customer_delight" sheetId="8" r:id="rId9"/>
+    <sheet name="Engineer_delight" sheetId="9" r:id="rId10"/>
+    <sheet name="Engineer_upskilling" sheetId="10" r:id="rId11"/>
+    <sheet name="Governance_customer" sheetId="11" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="777" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="75">
   <si>
     <t>id</t>
   </si>
@@ -316,7 +317,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -332,7 +333,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -650,18 +651,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2056A209-439C-471A-AC40-BB7C1896BCBF}">
   <dimension ref="C6:U183"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N154" workbookViewId="0">
-      <selection activeCell="Y164" sqref="X164:Y164"/>
+    <sheetView topLeftCell="A99" workbookViewId="0">
+      <selection activeCell="C113" sqref="C113:K123"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="18.3984375" customWidth="1"/>
-    <col min="11" max="11" width="22.265625" customWidth="1"/>
-    <col min="15" max="15" width="10.3984375" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" customWidth="1"/>
+    <col min="11" max="11" width="22.33203125" customWidth="1"/>
+    <col min="15" max="15" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="6" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
         <v>0</v>
       </c>
@@ -693,7 +694,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="8" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C8">
         <v>1</v>
       </c>
@@ -725,7 +726,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="9" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="9" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C9">
         <v>2</v>
       </c>
@@ -757,7 +758,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="10" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C10">
         <v>3</v>
       </c>
@@ -789,7 +790,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="11" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C11">
         <v>4</v>
       </c>
@@ -821,7 +822,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="12" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="12" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C12">
         <v>5</v>
       </c>
@@ -853,7 +854,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="13" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C13">
         <v>6</v>
       </c>
@@ -885,7 +886,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="14" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C14">
         <v>7</v>
       </c>
@@ -917,7 +918,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="15" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="15" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C15">
         <v>8</v>
       </c>
@@ -949,7 +950,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="16" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C16">
         <v>9</v>
       </c>
@@ -981,7 +982,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="24" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="24" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C24" t="s">
         <v>0</v>
       </c>
@@ -1013,7 +1014,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="26" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C26">
         <v>1</v>
       </c>
@@ -1045,7 +1046,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="27" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C27">
         <v>2</v>
       </c>
@@ -1077,7 +1078,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="28" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C28">
         <v>3</v>
       </c>
@@ -1109,7 +1110,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="29" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C29">
         <v>4</v>
       </c>
@@ -1141,7 +1142,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="30" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C30">
         <v>5</v>
       </c>
@@ -1173,7 +1174,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="31" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C31">
         <v>6</v>
       </c>
@@ -1205,7 +1206,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="32" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C32">
         <v>7</v>
       </c>
@@ -1237,7 +1238,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="33" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C33">
         <v>8</v>
       </c>
@@ -1269,7 +1270,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="34" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="34" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C34">
         <v>9</v>
       </c>
@@ -1301,7 +1302,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="41" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="41" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C41" t="s">
         <v>0</v>
       </c>
@@ -1333,7 +1334,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="43" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="43" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C43">
         <v>1</v>
       </c>
@@ -1365,7 +1366,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="44" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="44" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C44">
         <v>2</v>
       </c>
@@ -1397,7 +1398,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="45" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="45" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C45">
         <v>3</v>
       </c>
@@ -1429,7 +1430,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="46" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="46" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C46">
         <v>4</v>
       </c>
@@ -1461,7 +1462,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="47" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="47" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C47">
         <v>5</v>
       </c>
@@ -1493,7 +1494,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="48" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="48" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C48">
         <v>6</v>
       </c>
@@ -1525,7 +1526,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="49" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="49" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C49">
         <v>7</v>
       </c>
@@ -1557,7 +1558,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="50" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="50" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C50">
         <v>8</v>
       </c>
@@ -1589,7 +1590,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="51" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="51" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C51">
         <v>9</v>
       </c>
@@ -1621,7 +1622,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="58" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="58" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C58" t="s">
         <v>0</v>
       </c>
@@ -1653,7 +1654,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="60" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="60" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C60">
         <v>1</v>
       </c>
@@ -1685,7 +1686,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="61" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="61" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C61">
         <v>2</v>
       </c>
@@ -1717,7 +1718,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="62" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="62" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C62">
         <v>3</v>
       </c>
@@ -1749,7 +1750,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="63" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="63" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C63">
         <v>4</v>
       </c>
@@ -1781,7 +1782,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="64" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="64" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C64">
         <v>5</v>
       </c>
@@ -1813,7 +1814,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="65" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="65" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C65">
         <v>6</v>
       </c>
@@ -1845,7 +1846,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="66" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="66" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C66">
         <v>7</v>
       </c>
@@ -1877,7 +1878,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="67" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="67" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C67">
         <v>8</v>
       </c>
@@ -1909,7 +1910,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="68" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="68" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C68">
         <v>9</v>
       </c>
@@ -1941,7 +1942,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="113" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="113" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C113" t="s">
         <v>0</v>
       </c>
@@ -1973,7 +1974,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="115" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="115" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C115">
         <v>1</v>
       </c>
@@ -2005,7 +2006,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="116" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="116" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C116">
         <v>2</v>
       </c>
@@ -2037,7 +2038,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="117" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="117" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C117">
         <v>3</v>
       </c>
@@ -2069,7 +2070,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="118" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="118" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C118">
         <v>4</v>
       </c>
@@ -2101,7 +2102,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="119" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="119" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C119">
         <v>5</v>
       </c>
@@ -2133,7 +2134,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="120" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="120" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C120">
         <v>6</v>
       </c>
@@ -2165,7 +2166,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="121" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="121" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C121">
         <v>7</v>
       </c>
@@ -2197,7 +2198,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="122" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="122" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C122">
         <v>8</v>
       </c>
@@ -2229,7 +2230,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="123" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="123" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C123">
         <v>9</v>
       </c>
@@ -2261,7 +2262,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="128" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="128" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C128" t="s">
         <v>0</v>
       </c>
@@ -2293,7 +2294,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="130" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="130" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C130">
         <v>1</v>
       </c>
@@ -2325,7 +2326,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="131" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="131" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C131">
         <v>2</v>
       </c>
@@ -2357,7 +2358,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="132" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="132" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C132">
         <v>3</v>
       </c>
@@ -2389,7 +2390,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="133" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="133" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C133">
         <v>4</v>
       </c>
@@ -2421,7 +2422,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="134" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="134" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C134">
         <v>5</v>
       </c>
@@ -2453,7 +2454,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="135" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="135" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C135">
         <v>6</v>
       </c>
@@ -2485,7 +2486,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="136" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="136" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C136">
         <v>7</v>
       </c>
@@ -2517,7 +2518,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="137" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="137" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C137">
         <v>8</v>
       </c>
@@ -2549,7 +2550,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="138" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="138" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C138">
         <v>9</v>
       </c>
@@ -2581,7 +2582,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="144" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="144" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C144" t="s">
         <v>0</v>
       </c>
@@ -2613,7 +2614,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="146" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="146" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C146">
         <v>1</v>
       </c>
@@ -2645,7 +2646,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="147" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="147" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C147">
         <v>2</v>
       </c>
@@ -2677,7 +2678,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="148" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="148" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C148">
         <v>3</v>
       </c>
@@ -2709,7 +2710,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="149" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="149" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C149">
         <v>4</v>
       </c>
@@ -2741,7 +2742,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="150" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="150" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C150">
         <v>5</v>
       </c>
@@ -2773,7 +2774,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="151" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="151" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C151">
         <v>6</v>
       </c>
@@ -2805,7 +2806,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="152" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="152" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C152">
         <v>7</v>
       </c>
@@ -2837,7 +2838,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="153" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="153" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C153">
         <v>8</v>
       </c>
@@ -2869,7 +2870,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="154" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="154" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C154">
         <v>9</v>
       </c>
@@ -2901,7 +2902,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="159" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="159" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C159" t="s">
         <v>0</v>
       </c>
@@ -2933,7 +2934,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="161" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="161" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C161">
         <v>1</v>
       </c>
@@ -2965,7 +2966,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="162" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="162" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C162">
         <v>2</v>
       </c>
@@ -2997,7 +2998,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="163" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="163" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C163">
         <v>3</v>
       </c>
@@ -3029,7 +3030,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="164" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="164" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C164">
         <v>4</v>
       </c>
@@ -3061,7 +3062,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="165" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="165" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C165">
         <v>5</v>
       </c>
@@ -3093,7 +3094,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="166" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="166" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C166">
         <v>6</v>
       </c>
@@ -3125,7 +3126,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="167" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="167" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C167">
         <v>7</v>
       </c>
@@ -3157,7 +3158,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="168" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="168" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C168">
         <v>8</v>
       </c>
@@ -3189,7 +3190,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="169" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="169" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C169">
         <v>9</v>
       </c>
@@ -3221,7 +3222,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="173" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="173" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C173" t="s">
         <v>0</v>
       </c>
@@ -3253,7 +3254,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="175" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="175" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C175">
         <v>1</v>
       </c>
@@ -3285,7 +3286,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="176" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="176" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C176">
         <v>2</v>
       </c>
@@ -3317,7 +3318,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="177" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="177" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C177">
         <v>3</v>
       </c>
@@ -3349,7 +3350,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="178" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="178" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C178">
         <v>4</v>
       </c>
@@ -3381,7 +3382,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="179" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="179" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C179">
         <v>5</v>
       </c>
@@ -3413,7 +3414,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="180" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="180" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C180">
         <v>6</v>
       </c>
@@ -3445,7 +3446,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="181" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="181" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C181">
         <v>7</v>
       </c>
@@ -3477,7 +3478,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="182" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="182" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C182">
         <v>8</v>
       </c>
@@ -3509,7 +3510,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="183" spans="3:21" x14ac:dyDescent="0.45">
+    <row r="183" spans="3:21" x14ac:dyDescent="0.2">
       <c r="C183">
         <v>9</v>
       </c>
@@ -3548,6 +3549,95 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{845E186F-23E9-4636-B7BB-F09ADFC155D4}">
+  <dimension ref="E12:N17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12:N17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="12" spans="5:14" x14ac:dyDescent="0.2">
+      <c r="E12" t="s">
+        <v>0</v>
+      </c>
+      <c r="G12" t="s">
+        <v>1</v>
+      </c>
+      <c r="I12" t="s">
+        <v>2</v>
+      </c>
+      <c r="K12" t="s">
+        <v>3</v>
+      </c>
+      <c r="N12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="5:14" x14ac:dyDescent="0.2">
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
+        <v>64</v>
+      </c>
+      <c r="I14">
+        <v>76</v>
+      </c>
+      <c r="N14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="5:14" x14ac:dyDescent="0.2">
+      <c r="E15">
+        <v>2</v>
+      </c>
+      <c r="G15" t="s">
+        <v>65</v>
+      </c>
+      <c r="I15">
+        <v>76</v>
+      </c>
+      <c r="N15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="5:14" x14ac:dyDescent="0.2">
+      <c r="E16">
+        <v>3</v>
+      </c>
+      <c r="G16" t="s">
+        <v>66</v>
+      </c>
+      <c r="I16">
+        <v>60</v>
+      </c>
+      <c r="N16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="5:14" x14ac:dyDescent="0.2">
+      <c r="E17">
+        <v>4</v>
+      </c>
+      <c r="G17" t="s">
+        <v>67</v>
+      </c>
+      <c r="I17">
+        <v>60</v>
+      </c>
+      <c r="N17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65648BBE-0CD0-4610-BC69-5EEC5DB552DD}">
   <dimension ref="F14:O18"/>
   <sheetViews>
@@ -3555,9 +3645,9 @@
       <selection activeCell="F14" sqref="F14:O18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="14" spans="6:15" x14ac:dyDescent="0.45">
+    <row r="14" spans="6:15" x14ac:dyDescent="0.2">
       <c r="F14" t="s">
         <v>0</v>
       </c>
@@ -3574,7 +3664,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="6:15" x14ac:dyDescent="0.45">
+    <row r="16" spans="6:15" x14ac:dyDescent="0.2">
       <c r="F16">
         <v>1</v>
       </c>
@@ -3588,7 +3678,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="6:15" x14ac:dyDescent="0.45">
+    <row r="17" spans="6:15" x14ac:dyDescent="0.2">
       <c r="F17">
         <v>2</v>
       </c>
@@ -3602,7 +3692,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="6:15" x14ac:dyDescent="0.45">
+    <row r="18" spans="6:15" x14ac:dyDescent="0.2">
       <c r="F18">
         <v>3</v>
       </c>
@@ -3621,7 +3711,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94DD81D7-D221-42C9-849F-73FC0AD4452F}">
   <dimension ref="F14:O16"/>
   <sheetViews>
@@ -3629,9 +3719,9 @@
       <selection activeCell="X10" sqref="X10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="14" spans="6:15" x14ac:dyDescent="0.45">
+    <row r="14" spans="6:15" x14ac:dyDescent="0.2">
       <c r="F14" t="s">
         <v>0</v>
       </c>
@@ -3648,7 +3738,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="6:15" x14ac:dyDescent="0.45">
+    <row r="16" spans="6:15" x14ac:dyDescent="0.2">
       <c r="F16">
         <v>1</v>
       </c>
@@ -3675,9 +3765,9 @@
       <selection activeCell="D7" sqref="D7:M12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="7" spans="4:13" x14ac:dyDescent="0.45">
+    <row r="7" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D7" t="s">
         <v>0</v>
       </c>
@@ -3694,7 +3784,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="4:13" x14ac:dyDescent="0.45">
+    <row r="9" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D9">
         <v>1</v>
       </c>
@@ -3708,7 +3798,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="4:13" x14ac:dyDescent="0.45">
+    <row r="10" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D10">
         <v>2</v>
       </c>
@@ -3725,7 +3815,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="4:13" x14ac:dyDescent="0.45">
+    <row r="11" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D11">
         <v>3</v>
       </c>
@@ -3742,7 +3832,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="4:13" x14ac:dyDescent="0.45">
+    <row r="12" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D12">
         <v>4</v>
       </c>
@@ -3772,14 +3862,14 @@
       <selection activeCell="P19" sqref="P19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" width="38.53125" customWidth="1"/>
-    <col min="7" max="7" width="13.59765625" customWidth="1"/>
-    <col min="10" max="10" width="29.9296875" customWidth="1"/>
+    <col min="6" max="6" width="38.5" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" customWidth="1"/>
+    <col min="10" max="10" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="4:13" x14ac:dyDescent="0.45">
+    <row r="7" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D7" t="s">
         <v>0</v>
       </c>
@@ -3796,7 +3886,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="4:13" x14ac:dyDescent="0.45">
+    <row r="9" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D9">
         <v>1</v>
       </c>
@@ -3810,7 +3900,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="4:13" x14ac:dyDescent="0.45">
+    <row r="10" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D10">
         <v>2</v>
       </c>
@@ -3827,7 +3917,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="4:13" x14ac:dyDescent="0.45">
+    <row r="11" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D11">
         <v>3</v>
       </c>
@@ -3838,7 +3928,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="4:13" x14ac:dyDescent="0.45">
+    <row r="12" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D12">
         <v>4</v>
       </c>
@@ -3855,7 +3945,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="4:13" x14ac:dyDescent="0.45">
+    <row r="13" spans="4:13" x14ac:dyDescent="0.2">
       <c r="D13">
         <v>5</v>
       </c>
@@ -3878,6 +3968,89 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37C39950-1442-CB41-BC37-4003DCB3CA27}">
+  <dimension ref="D7:L11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B6" zoomScale="171" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="7" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="D7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F7" t="s">
+        <v>1</v>
+      </c>
+      <c r="H7" t="s">
+        <v>2</v>
+      </c>
+      <c r="J7" t="s">
+        <v>3</v>
+      </c>
+      <c r="L7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9">
+        <v>6</v>
+      </c>
+      <c r="J9" t="s">
+        <v>7</v>
+      </c>
+      <c r="L9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="F10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H10">
+        <v>4</v>
+      </c>
+      <c r="J10" t="s">
+        <v>7</v>
+      </c>
+      <c r="L10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="F11" t="s">
+        <v>6</v>
+      </c>
+      <c r="H11">
+        <v>5</v>
+      </c>
+      <c r="J11" t="s">
+        <v>7</v>
+      </c>
+      <c r="L11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CB0321B-1694-4805-B7CB-5AE863A01116}">
   <dimension ref="C16:L20"/>
   <sheetViews>
@@ -3885,15 +4058,15 @@
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="5" max="5" width="38" customWidth="1"/>
-    <col min="6" max="6" width="8.796875" customWidth="1"/>
+    <col min="6" max="6" width="8.83203125" customWidth="1"/>
     <col min="9" max="9" width="30.6640625" customWidth="1"/>
-    <col min="12" max="12" width="22.265625" customWidth="1"/>
+    <col min="12" max="12" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="16" spans="3:12" x14ac:dyDescent="0.45">
+    <row r="16" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C16" t="s">
         <v>0</v>
       </c>
@@ -3910,7 +4083,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="3:9" x14ac:dyDescent="0.45">
+    <row r="18" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C18">
         <v>1</v>
       </c>
@@ -3924,7 +4097,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="3:9" x14ac:dyDescent="0.45">
+    <row r="19" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C19">
         <v>2</v>
       </c>
@@ -3938,7 +4111,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="3:9" x14ac:dyDescent="0.45">
+    <row r="20" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C20">
         <v>3</v>
       </c>
@@ -3958,17 +4131,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5C7C0CD-5A0A-4AB9-A8FE-8201FB8719E1}">
   <dimension ref="E14:N18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14:N18"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="14" spans="5:14" x14ac:dyDescent="0.45">
+    <row r="14" spans="5:14" x14ac:dyDescent="0.2">
       <c r="E14" t="s">
         <v>0</v>
       </c>
@@ -3985,7 +4158,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="5:14" x14ac:dyDescent="0.45">
+    <row r="16" spans="5:14" x14ac:dyDescent="0.2">
       <c r="E16">
         <v>1</v>
       </c>
@@ -4002,7 +4175,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="5:14" x14ac:dyDescent="0.45">
+    <row r="17" spans="5:14" x14ac:dyDescent="0.2">
       <c r="E17">
         <v>2</v>
       </c>
@@ -4019,7 +4192,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="5:14" x14ac:dyDescent="0.45">
+    <row r="18" spans="5:14" x14ac:dyDescent="0.2">
       <c r="E18">
         <v>3</v>
       </c>
@@ -4038,7 +4211,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48201469-AAFD-45E5-9709-A98526EE2BE7}">
   <dimension ref="F14:O18"/>
   <sheetViews>
@@ -4046,9 +4219,9 @@
       <selection activeCell="F14" sqref="F14:O18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="14" spans="6:15" x14ac:dyDescent="0.45">
+    <row r="14" spans="6:15" x14ac:dyDescent="0.2">
       <c r="F14" t="s">
         <v>0</v>
       </c>
@@ -4065,7 +4238,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="6:15" x14ac:dyDescent="0.45">
+    <row r="16" spans="6:15" x14ac:dyDescent="0.2">
       <c r="F16">
         <v>1</v>
       </c>
@@ -4079,7 +4252,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="6:15" x14ac:dyDescent="0.45">
+    <row r="17" spans="6:15" x14ac:dyDescent="0.2">
       <c r="F17">
         <v>2</v>
       </c>
@@ -4093,7 +4266,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="6:15" x14ac:dyDescent="0.45">
+    <row r="18" spans="6:15" x14ac:dyDescent="0.2">
       <c r="F18">
         <v>3</v>
       </c>
@@ -4112,7 +4285,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C54E2ED4-78AC-4FA7-B729-F0C6DF47B945}">
   <dimension ref="E12:N16"/>
   <sheetViews>
@@ -4120,9 +4293,9 @@
       <selection activeCell="E12" sqref="E12:N16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="12" spans="5:14" x14ac:dyDescent="0.45">
+    <row r="12" spans="5:14" x14ac:dyDescent="0.2">
       <c r="E12" t="s">
         <v>0</v>
       </c>
@@ -4139,7 +4312,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="5:14" x14ac:dyDescent="0.45">
+    <row r="14" spans="5:14" x14ac:dyDescent="0.2">
       <c r="E14">
         <v>1</v>
       </c>
@@ -4153,7 +4326,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="5:14" x14ac:dyDescent="0.45">
+    <row r="15" spans="5:14" x14ac:dyDescent="0.2">
       <c r="E15">
         <v>2</v>
       </c>
@@ -4167,7 +4340,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="5:14" x14ac:dyDescent="0.45">
+    <row r="16" spans="5:14" x14ac:dyDescent="0.2">
       <c r="E16">
         <v>3</v>
       </c>
@@ -4186,7 +4359,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44332FF3-929A-46EC-9CF8-88538010FE32}">
   <dimension ref="C11:L14"/>
   <sheetViews>
@@ -4194,9 +4367,9 @@
       <selection activeCell="C11" sqref="C11:L14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="11" spans="3:12" x14ac:dyDescent="0.45">
+    <row r="11" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C11" t="s">
         <v>0</v>
       </c>
@@ -4213,7 +4386,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="3:12" x14ac:dyDescent="0.45">
+    <row r="13" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C13">
         <v>1</v>
       </c>
@@ -4227,7 +4400,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="3:12" x14ac:dyDescent="0.45">
+    <row r="14" spans="3:12" x14ac:dyDescent="0.2">
       <c r="C14">
         <v>2</v>
       </c>
@@ -4244,93 +4417,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{845E186F-23E9-4636-B7BB-F09ADFC155D4}">
-  <dimension ref="E12:N17"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12:N17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <sheetData>
-    <row r="12" spans="5:14" x14ac:dyDescent="0.45">
-      <c r="E12" t="s">
-        <v>0</v>
-      </c>
-      <c r="G12" t="s">
-        <v>1</v>
-      </c>
-      <c r="I12" t="s">
-        <v>2</v>
-      </c>
-      <c r="K12" t="s">
-        <v>3</v>
-      </c>
-      <c r="N12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="5:14" x14ac:dyDescent="0.45">
-      <c r="E14">
-        <v>1</v>
-      </c>
-      <c r="G14" t="s">
-        <v>64</v>
-      </c>
-      <c r="I14">
-        <v>76</v>
-      </c>
-      <c r="N14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="5:14" x14ac:dyDescent="0.45">
-      <c r="E15">
-        <v>2</v>
-      </c>
-      <c r="G15" t="s">
-        <v>65</v>
-      </c>
-      <c r="I15">
-        <v>76</v>
-      </c>
-      <c r="N15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="5:14" x14ac:dyDescent="0.45">
-      <c r="E16">
-        <v>3</v>
-      </c>
-      <c r="G16" t="s">
-        <v>66</v>
-      </c>
-      <c r="I16">
-        <v>60</v>
-      </c>
-      <c r="N16" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="5:14" x14ac:dyDescent="0.45">
-      <c r="E17">
-        <v>4</v>
-      </c>
-      <c r="G17" t="s">
-        <v>67</v>
-      </c>
-      <c r="I17">
-        <v>60</v>
-      </c>
-      <c r="N17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Operations customer specific done! Without ss
</commit_message>
<xml_diff>
--- a/data/dB.xlsx
+++ b/data/dB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brahamjeet/HCLTech_Dashboard/Dashboard/Dashboard-HCLTech/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{797E32F8-E407-3C40-ABBA-2FAA64F0AA36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EFEC4B6-6E2B-0F4D-BB79-D26B430484B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="3" xr2:uid="{9CAA6723-E93B-4360-9D44-745D8D6BCC11}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="7" xr2:uid="{9CAA6723-E93B-4360-9D44-745D8D6BCC11}"/>
   </bookViews>
   <sheets>
     <sheet name="Financials" sheetId="1" r:id="rId1"/>
@@ -20,11 +20,12 @@
     <sheet name="Thought_leadership" sheetId="4" r:id="rId5"/>
     <sheet name="North_star" sheetId="5" r:id="rId6"/>
     <sheet name="GTM_improvement" sheetId="6" r:id="rId7"/>
-    <sheet name="Operations_hcltech" sheetId="7" r:id="rId8"/>
-    <sheet name="Customer_delight" sheetId="8" r:id="rId9"/>
-    <sheet name="Engineer_delight" sheetId="9" r:id="rId10"/>
-    <sheet name="Engineer_upskilling" sheetId="10" r:id="rId11"/>
-    <sheet name="Governance_customer" sheetId="11" r:id="rId12"/>
+    <sheet name="Operations_customer" sheetId="13" r:id="rId8"/>
+    <sheet name="Operations_hcltech" sheetId="7" r:id="rId9"/>
+    <sheet name="Customer_delight" sheetId="8" r:id="rId10"/>
+    <sheet name="Engineer_delight" sheetId="9" r:id="rId11"/>
+    <sheet name="Engineer_upskilling" sheetId="10" r:id="rId12"/>
+    <sheet name="Governance_customer" sheetId="11" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="77">
   <si>
     <t>id</t>
   </si>
@@ -272,6 +273,12 @@
   </si>
   <si>
     <t>testing</t>
+  </si>
+  <si>
+    <t>hyt</t>
+  </si>
+  <si>
+    <t>yhy</t>
   </si>
 </sst>
 </file>
@@ -3549,6 +3556,66 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44332FF3-929A-46EC-9CF8-88538010FE32}">
+  <dimension ref="C11:L14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11:L14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="11" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>2</v>
+      </c>
+      <c r="I11" t="s">
+        <v>3</v>
+      </c>
+      <c r="L11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="E13" t="s">
+        <v>62</v>
+      </c>
+      <c r="G13">
+        <v>85</v>
+      </c>
+      <c r="L13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="E14" t="s">
+        <v>63</v>
+      </c>
+      <c r="G14">
+        <v>6.3</v>
+      </c>
+      <c r="L14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{845E186F-23E9-4636-B7BB-F09ADFC155D4}">
   <dimension ref="E12:N17"/>
   <sheetViews>
@@ -3637,7 +3704,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65648BBE-0CD0-4610-BC69-5EEC5DB552DD}">
   <dimension ref="F14:O18"/>
   <sheetViews>
@@ -3711,7 +3778,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94DD81D7-D221-42C9-849F-73FC0AD4452F}">
   <dimension ref="F14:O16"/>
   <sheetViews>
@@ -3971,7 +4038,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37C39950-1442-CB41-BC37-4003DCB3CA27}">
   <dimension ref="D7:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B6" zoomScale="171" workbookViewId="0">
+    <sheetView topLeftCell="B6" zoomScale="171" workbookViewId="0">
       <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
@@ -4286,6 +4353,89 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1DA016A-4554-ED4B-A2AE-AB37C0AD6BFF}">
+  <dimension ref="C6:L10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="6" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>2</v>
+      </c>
+      <c r="I6" t="s">
+        <v>3</v>
+      </c>
+      <c r="L6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8">
+        <v>55</v>
+      </c>
+      <c r="I8" t="s">
+        <v>75</v>
+      </c>
+      <c r="L8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9">
+        <v>7</v>
+      </c>
+      <c r="I9" t="s">
+        <v>75</v>
+      </c>
+      <c r="L9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="3:12" x14ac:dyDescent="0.2">
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="E10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G10">
+        <v>99</v>
+      </c>
+      <c r="I10" t="s">
+        <v>76</v>
+      </c>
+      <c r="L10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C54E2ED4-78AC-4FA7-B729-F0C6DF47B945}">
   <dimension ref="E12:N16"/>
   <sheetViews>
@@ -4357,64 +4507,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44332FF3-929A-46EC-9CF8-88538010FE32}">
-  <dimension ref="C11:L14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11:L14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="11" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C11" t="s">
-        <v>0</v>
-      </c>
-      <c r="E11" t="s">
-        <v>1</v>
-      </c>
-      <c r="G11" t="s">
-        <v>2</v>
-      </c>
-      <c r="I11" t="s">
-        <v>3</v>
-      </c>
-      <c r="L11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="E13" t="s">
-        <v>62</v>
-      </c>
-      <c r="G13">
-        <v>85</v>
-      </c>
-      <c r="L13" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="3:12" x14ac:dyDescent="0.2">
-      <c r="C14">
-        <v>2</v>
-      </c>
-      <c r="E14" t="s">
-        <v>63</v>
-      </c>
-      <c r="G14">
-        <v>6.3</v>
-      </c>
-      <c r="L14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Dex page done! Without ss
</commit_message>
<xml_diff>
--- a/data/dB.xlsx
+++ b/data/dB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brahamjeet/HCLTech_Dashboard/Dashboard/Dashboard-HCLTech/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EFEC4B6-6E2B-0F4D-BB79-D26B430484B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72AC5747-7BEC-0945-853C-73E62EE01052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="7" xr2:uid="{9CAA6723-E93B-4360-9D44-745D8D6BCC11}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="10" xr2:uid="{9CAA6723-E93B-4360-9D44-745D8D6BCC11}"/>
   </bookViews>
   <sheets>
     <sheet name="Financials" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,10 @@
     <sheet name="Operations_customer" sheetId="13" r:id="rId8"/>
     <sheet name="Operations_hcltech" sheetId="7" r:id="rId9"/>
     <sheet name="Customer_delight" sheetId="8" r:id="rId10"/>
-    <sheet name="Engineer_delight" sheetId="9" r:id="rId11"/>
-    <sheet name="Engineer_upskilling" sheetId="10" r:id="rId12"/>
-    <sheet name="Governance_customer" sheetId="11" r:id="rId13"/>
+    <sheet name="dex" sheetId="14" r:id="rId11"/>
+    <sheet name="Engineer_delight" sheetId="9" r:id="rId12"/>
+    <sheet name="Engineer_upskilling" sheetId="10" r:id="rId13"/>
+    <sheet name="Governance_customer" sheetId="11" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="819" uniqueCount="77">
   <si>
     <t>id</t>
   </si>
@@ -3616,6 +3617,89 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6187DF87-1759-D14C-B4F9-22EA9BC81DDB}">
+  <dimension ref="D8:L12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="8" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="D8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>1</v>
+      </c>
+      <c r="H8" t="s">
+        <v>2</v>
+      </c>
+      <c r="J8" t="s">
+        <v>3</v>
+      </c>
+      <c r="L8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
+        <v>4</v>
+      </c>
+      <c r="H10">
+        <v>54</v>
+      </c>
+      <c r="J10" t="s">
+        <v>7</v>
+      </c>
+      <c r="L10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="F11" t="s">
+        <v>5</v>
+      </c>
+      <c r="H11">
+        <v>55</v>
+      </c>
+      <c r="J11" t="s">
+        <v>7</v>
+      </c>
+      <c r="L11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="4:12" x14ac:dyDescent="0.2">
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="F12" t="s">
+        <v>6</v>
+      </c>
+      <c r="H12">
+        <v>89</v>
+      </c>
+      <c r="J12" t="s">
+        <v>7</v>
+      </c>
+      <c r="L12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{845E186F-23E9-4636-B7BB-F09ADFC155D4}">
   <dimension ref="E12:N17"/>
   <sheetViews>
@@ -3704,7 +3788,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65648BBE-0CD0-4610-BC69-5EEC5DB552DD}">
   <dimension ref="F14:O18"/>
   <sheetViews>
@@ -3778,7 +3862,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94DD81D7-D221-42C9-849F-73FC0AD4452F}">
   <dimension ref="F14:O16"/>
   <sheetViews>
@@ -4038,8 +4122,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37C39950-1442-CB41-BC37-4003DCB3CA27}">
   <dimension ref="D7:L11"/>
   <sheetViews>
-    <sheetView topLeftCell="B6" zoomScale="171" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView topLeftCell="C6" zoomScale="171" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4069,7 +4153,7 @@
         <v>4</v>
       </c>
       <c r="H9">
-        <v>6</v>
+        <v>88</v>
       </c>
       <c r="J9" t="s">
         <v>7</v>
@@ -4086,7 +4170,7 @@
         <v>5</v>
       </c>
       <c r="H10">
-        <v>4</v>
+        <v>85</v>
       </c>
       <c r="J10" t="s">
         <v>7</v>
@@ -4103,7 +4187,7 @@
         <v>6</v>
       </c>
       <c r="H11">
-        <v>5</v>
+        <v>66</v>
       </c>
       <c r="J11" t="s">
         <v>7</v>
@@ -4203,7 +4287,7 @@
   <dimension ref="E14:N18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="L44" sqref="L44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4356,8 +4440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1DA016A-4554-ED4B-A2AE-AB37C0AD6BFF}">
   <dimension ref="C6:L10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Governance internal facing done!
Without ss
</commit_message>
<xml_diff>
--- a/data/dB.xlsx
+++ b/data/dB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brahamjeet/HCLTech_Dashboard/Dashboard/Dashboard-HCLTech/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72AC5747-7BEC-0945-853C-73E62EE01052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3697087-2DEB-D94E-AB64-02D6A06FB057}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="10" xr2:uid="{9CAA6723-E93B-4360-9D44-745D8D6BCC11}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" firstSheet="6" activeTab="14" xr2:uid="{9CAA6723-E93B-4360-9D44-745D8D6BCC11}"/>
   </bookViews>
   <sheets>
     <sheet name="Financials" sheetId="1" r:id="rId1"/>
@@ -27,6 +27,7 @@
     <sheet name="Engineer_delight" sheetId="9" r:id="rId12"/>
     <sheet name="Engineer_upskilling" sheetId="10" r:id="rId13"/>
     <sheet name="Governance_customer" sheetId="11" r:id="rId14"/>
+    <sheet name="Governance_internal" sheetId="15" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="819" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="77">
   <si>
     <t>id</t>
   </si>
@@ -3620,7 +3621,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6187DF87-1759-D14C-B4F9-22EA9BC81DDB}">
   <dimension ref="D8:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
@@ -3901,6 +3902,89 @@
       </c>
       <c r="O16" t="s">
         <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0830408D-A864-0B43-858E-9BA2A19A75AF}">
+  <dimension ref="C7:K11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N15" sqref="N15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="7" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7" t="s">
+        <v>2</v>
+      </c>
+      <c r="I7" t="s">
+        <v>3</v>
+      </c>
+      <c r="K7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9">
+        <v>6</v>
+      </c>
+      <c r="I9" t="s">
+        <v>7</v>
+      </c>
+      <c r="K9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10">
+        <v>4</v>
+      </c>
+      <c r="I10" t="s">
+        <v>7</v>
+      </c>
+      <c r="K10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="E11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11">
+        <v>5</v>
+      </c>
+      <c r="I11" t="s">
+        <v>7</v>
+      </c>
+      <c r="K11" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>